<commit_message>
Videre med sigmoid neuron. OBS! Eksemplet skal ændres.
</commit_message>
<xml_diff>
--- a/materialer/sigmoid_neuron/_Geogebra/test_sigmoid_neuron_eks1.xlsx
+++ b/materialer/sigmoid_neuron/_Geogebra/test_sigmoid_neuron_eks1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Documents\GitHub\aalborg-intelligence.github.io\materialer\sigmoid_neuron\_Geogebra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09333D60-758B-47FD-8C26-38190869167B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A195A6-3B8D-42F9-9130-E4BEEA7FB929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="34620" windowHeight="13900" xr2:uid="{DBE89888-1415-442E-86F8-4AC29F924318}"/>
+    <workbookView xWindow="41410" yWindow="870" windowWidth="11800" windowHeight="11440" xr2:uid="{DBE89888-1415-442E-86F8-4AC29F924318}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>var1</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>target</t>
+  </si>
+  <si>
+    <t>target01</t>
   </si>
 </sst>
 </file>
@@ -416,15 +419,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157CB2BA-E092-4A8C-A8CF-5A7D6E5566F0}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,8 +437,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>-0.5</v>
       </c>
@@ -445,8 +451,11 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>-0.3</v>
       </c>
@@ -456,8 +465,11 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>-0.1</v>
       </c>
@@ -467,8 +479,11 @@
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.1</v>
       </c>
@@ -478,8 +493,11 @@
       <c r="C5">
         <v>-1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>-0.1</v>
       </c>
@@ -489,8 +507,11 @@
       <c r="C6">
         <v>-1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0.1</v>
       </c>
@@ -499,6 +520,9 @@
       </c>
       <c r="C7">
         <v>-1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>